<commit_message>
avance e reporte quinceles
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaBalanceEnergia.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaBalanceEnergia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SP\UNNA-App\AppOperacionalReporte\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\diario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21DB4B4-776F-473D-AD89-2B04724EA6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91066975-D84F-41B1-BC16-CF135BBF1683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="445" xr2:uid="{9E40B278-673A-417E-9A41-08ACE2830EAA}"/>
   </bookViews>
@@ -209,7 +209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="112">
   <si>
     <t>Versión / Fecha</t>
   </si>
@@ -564,7 +564,7 @@
     <numFmt numFmtId="164" formatCode="[$-280A]dddd\ d&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Arial"/>
@@ -670,6 +670,23 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -870,7 +887,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="145">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1049,20 +1066,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1116,9 +1120,6 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1152,17 +1153,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1178,14 +1169,47 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="18" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1211,7 +1235,13 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1220,58 +1250,13 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1286,6 +1271,48 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="18" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="18" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1295,6 +1322,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1311,15 +1343,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>728789</xdr:colOff>
+      <xdr:colOff>281114</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>56030</xdr:rowOff>
+      <xdr:rowOff>65555</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>767241</xdr:colOff>
+      <xdr:colOff>823830</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>139742</xdr:rowOff>
+      <xdr:rowOff>149267</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1347,8 +1379,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="784818" y="56030"/>
-          <a:ext cx="2279628" cy="845712"/>
+          <a:off x="871664" y="65555"/>
+          <a:ext cx="2276266" cy="845712"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1376,7 +1408,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>168088</xdr:colOff>
+      <xdr:colOff>168089</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>152681</xdr:rowOff>
     </xdr:to>
@@ -30356,14 +30388,14 @@
   </sheetPr>
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScale="85" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42:L44"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="130" zoomScaleNormal="70" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" style="1" customWidth="1"/>
     <col min="3" max="3" width="23.21875" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.109375" style="1" customWidth="1"/>
@@ -30379,106 +30411,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="133"/>
-      <c r="B1" s="133"/>
-      <c r="C1" s="133"/>
-      <c r="D1" s="136" t="s">
+      <c r="A1" s="131"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="134" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="136"/>
-      <c r="J1" s="136"/>
-      <c r="K1" s="137" t="s">
+      <c r="E1" s="134"/>
+      <c r="F1" s="134"/>
+      <c r="G1" s="134"/>
+      <c r="H1" s="134"/>
+      <c r="I1" s="134"/>
+      <c r="J1" s="134"/>
+      <c r="K1" s="127" t="s">
         <v>67</v>
       </c>
-      <c r="L1" s="138"/>
-      <c r="M1" s="138"/>
-      <c r="N1" s="139"/>
+      <c r="L1" s="128"/>
+      <c r="M1" s="128"/>
+      <c r="N1" s="129"/>
     </row>
     <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="133"/>
-      <c r="B2" s="133"/>
-      <c r="C2" s="133"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
-      <c r="H2" s="136"/>
-      <c r="I2" s="136"/>
-      <c r="J2" s="136"/>
-      <c r="K2" s="116" t="s">
+      <c r="A2" s="131"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="143" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="117"/>
-      <c r="M2" s="117"/>
-      <c r="N2" s="118"/>
+      <c r="L2" s="122"/>
+      <c r="M2" s="122"/>
+      <c r="N2" s="123"/>
     </row>
     <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="133"/>
-      <c r="B3" s="133"/>
-      <c r="C3" s="133"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="136"/>
-      <c r="F3" s="136"/>
-      <c r="G3" s="136"/>
-      <c r="H3" s="136"/>
-      <c r="I3" s="136"/>
-      <c r="J3" s="136"/>
-      <c r="K3" s="119" t="s">
+      <c r="A3" s="131"/>
+      <c r="B3" s="131"/>
+      <c r="C3" s="131"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
+      <c r="H3" s="134"/>
+      <c r="I3" s="134"/>
+      <c r="J3" s="134"/>
+      <c r="K3" s="125" t="s">
         <v>68</v>
       </c>
-      <c r="L3" s="120"/>
-      <c r="M3" s="120"/>
-      <c r="N3" s="121"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="126"/>
     </row>
     <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="133"/>
-      <c r="B4" s="133"/>
-      <c r="C4" s="133"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
-      <c r="F4" s="136"/>
-      <c r="G4" s="136"/>
-      <c r="H4" s="136"/>
-      <c r="I4" s="136"/>
-      <c r="J4" s="136"/>
-      <c r="K4" s="122" t="s">
+      <c r="A4" s="131"/>
+      <c r="B4" s="131"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="134"/>
+      <c r="E4" s="134"/>
+      <c r="F4" s="134"/>
+      <c r="G4" s="134"/>
+      <c r="H4" s="134"/>
+      <c r="I4" s="134"/>
+      <c r="J4" s="134"/>
+      <c r="K4" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="123"/>
-      <c r="M4" s="117" t="s">
+      <c r="L4" s="121"/>
+      <c r="M4" s="122" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="118"/>
-      <c r="O4" s="100"/>
+      <c r="N4" s="123"/>
+      <c r="O4" s="90"/>
     </row>
     <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="133"/>
-      <c r="B5" s="133"/>
-      <c r="C5" s="133"/>
-      <c r="D5" s="136"/>
-      <c r="E5" s="136"/>
-      <c r="F5" s="136"/>
-      <c r="G5" s="136"/>
-      <c r="H5" s="136"/>
-      <c r="I5" s="136"/>
-      <c r="J5" s="136"/>
-      <c r="K5" s="117" t="s">
+      <c r="A5" s="131"/>
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="134"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="134"/>
+      <c r="H5" s="134"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
+      <c r="K5" s="122" t="s">
         <v>69</v>
       </c>
-      <c r="L5" s="117"/>
-      <c r="M5" s="119" t="s">
+      <c r="L5" s="122"/>
+      <c r="M5" s="125" t="s">
         <v>70</v>
       </c>
-      <c r="N5" s="121"/>
+      <c r="N5" s="126"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="102"/>
-      <c r="B6" s="101"/>
-      <c r="C6" s="101"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="91"/>
+      <c r="C6" s="91"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -30492,7 +30524,7 @@
       <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:15" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="100"/>
+      <c r="A7" s="90"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="5" t="s">
@@ -30510,7 +30542,7 @@
       <c r="N7" s="7"/>
     </row>
     <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="100"/>
+      <c r="A8" s="90"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="6"/>
@@ -30528,7 +30560,7 @@
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="100"/>
+      <c r="A9" s="90"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="6"/>
@@ -30544,13 +30576,13 @@
       <c r="N9" s="7"/>
     </row>
     <row r="10" spans="1:15" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="103"/>
+      <c r="A10" s="93"/>
       <c r="B10" s="17"/>
       <c r="G10" s="18"/>
       <c r="H10" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="60" t="s">
+      <c r="I10" s="104" t="s">
         <v>50</v>
       </c>
       <c r="L10" s="21"/>
@@ -30558,7 +30590,7 @@
       <c r="N10" s="56"/>
     </row>
     <row r="11" spans="1:15" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="103"/>
+      <c r="A11" s="93"/>
       <c r="B11" s="19"/>
       <c r="C11" s="17"/>
       <c r="E11" s="17"/>
@@ -30573,7 +30605,7 @@
       <c r="N11" s="56"/>
     </row>
     <row r="12" spans="1:15" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="103"/>
+      <c r="A12" s="93"/>
       <c r="B12" s="22"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -30587,7 +30619,7 @@
       <c r="N12" s="56"/>
     </row>
     <row r="13" spans="1:15" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="103"/>
+      <c r="A13" s="93"/>
       <c r="B13" s="23"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -30598,82 +30630,82 @@
       <c r="N13" s="56"/>
     </row>
     <row r="14" spans="1:15" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A14" s="103"/>
+      <c r="A14" s="93"/>
       <c r="B14" s="24"/>
-      <c r="C14" s="134" t="s">
+      <c r="C14" s="132" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="107" t="s">
+      <c r="D14" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="135" t="s">
+      <c r="E14" s="133" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="107" t="s">
+      <c r="F14" s="108" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="107" t="s">
+      <c r="G14" s="108" t="s">
         <v>11</v>
       </c>
       <c r="H14" s="25"/>
       <c r="I14" s="24"/>
-      <c r="J14" s="80" t="s">
+      <c r="J14" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="K14" s="80" t="s">
+      <c r="K14" s="75" t="s">
         <v>13</v>
       </c>
       <c r="N14" s="56"/>
     </row>
     <row r="15" spans="1:15" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="103"/>
+      <c r="A15" s="93"/>
       <c r="B15" s="24"/>
-      <c r="C15" s="134"/>
-      <c r="D15" s="107"/>
-      <c r="E15" s="135"/>
-      <c r="F15" s="107"/>
-      <c r="G15" s="107"/>
+      <c r="C15" s="132"/>
+      <c r="D15" s="108"/>
+      <c r="E15" s="133"/>
+      <c r="F15" s="108"/>
+      <c r="G15" s="108"/>
       <c r="H15" s="17"/>
-      <c r="I15" s="82" t="s">
+      <c r="I15" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="J15" s="83" t="s">
+      <c r="J15" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="K15" s="83" t="s">
+      <c r="K15" s="103" t="s">
         <v>56</v>
       </c>
       <c r="L15" s="46"/>
       <c r="N15" s="56"/>
     </row>
     <row r="16" spans="1:15" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="103"/>
+      <c r="A16" s="93"/>
       <c r="B16" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="127" t="s">
+      <c r="C16" s="135" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="129" t="s">
+      <c r="D16" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="131" t="s">
+      <c r="E16" s="139" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="129" t="s">
+      <c r="F16" s="141" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="125" t="s">
+      <c r="G16" s="139" t="s">
         <v>41</v>
       </c>
       <c r="H16" s="17"/>
-      <c r="I16" s="82" t="s">
+      <c r="I16" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="J16" s="83" t="s">
+      <c r="J16" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="K16" s="83" t="s">
+      <c r="K16" s="103" t="s">
         <v>58</v>
       </c>
       <c r="L16" s="47"/>
@@ -30681,21 +30713,21 @@
       <c r="N16" s="56"/>
     </row>
     <row r="17" spans="1:14" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="103"/>
-      <c r="B17" s="115"/>
-      <c r="C17" s="128"/>
-      <c r="D17" s="130"/>
-      <c r="E17" s="132"/>
-      <c r="F17" s="130"/>
-      <c r="G17" s="126"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="108"/>
+      <c r="C17" s="136"/>
+      <c r="D17" s="138"/>
+      <c r="E17" s="140"/>
+      <c r="F17" s="142"/>
+      <c r="G17" s="140"/>
       <c r="H17" s="17"/>
-      <c r="I17" s="82" t="s">
+      <c r="I17" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="J17" s="83" t="s">
+      <c r="J17" s="103" t="s">
         <v>59</v>
       </c>
-      <c r="K17" s="83" t="s">
+      <c r="K17" s="103" t="s">
         <v>60</v>
       </c>
       <c r="L17" s="47"/>
@@ -30703,23 +30735,33 @@
       <c r="N17" s="56"/>
     </row>
     <row r="18" spans="1:14" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="103"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="65"/>
+      <c r="A18" s="93"/>
+      <c r="B18" s="108"/>
+      <c r="C18" s="99" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="100" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="101" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="100" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="102" t="s">
+        <v>41</v>
+      </c>
       <c r="H18" s="17"/>
-      <c r="I18" s="66"/>
-      <c r="J18" s="67"/>
-      <c r="K18" s="67"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="62"/>
+      <c r="K18" s="62"/>
       <c r="L18" s="47"/>
       <c r="M18" s="37"/>
       <c r="N18" s="56"/>
     </row>
     <row r="19" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="103"/>
+      <c r="A19" s="93"/>
       <c r="B19" s="26"/>
       <c r="C19" s="27"/>
       <c r="D19" s="28"/>
@@ -30734,14 +30776,14 @@
       <c r="N19" s="56"/>
     </row>
     <row r="20" spans="1:14" s="45" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="103"/>
+      <c r="A20" s="93"/>
       <c r="B20" s="32"/>
       <c r="H20" s="33"/>
       <c r="L20" s="48"/>
       <c r="N20" s="56"/>
     </row>
     <row r="21" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="103"/>
+      <c r="A21" s="93"/>
       <c r="B21" s="34"/>
       <c r="C21" s="19"/>
       <c r="D21" s="35"/>
@@ -30749,10 +30791,10 @@
       <c r="F21" s="33"/>
       <c r="G21" s="33"/>
       <c r="H21" s="33"/>
-      <c r="I21" s="84" t="s">
+      <c r="I21" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="J21" s="85" t="s">
+      <c r="J21" s="79" t="s">
         <v>42</v>
       </c>
       <c r="K21" s="49"/>
@@ -30760,64 +30802,67 @@
       <c r="N21" s="56"/>
     </row>
     <row r="22" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="103"/>
+      <c r="A22" s="93"/>
       <c r="B22" s="36"/>
       <c r="E22" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="I22" s="84" t="s">
+      <c r="I22" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="J22" s="99" t="s">
+      <c r="J22" s="107" t="s">
         <v>61</v>
       </c>
       <c r="K22" s="48"/>
       <c r="N22" s="56"/>
     </row>
     <row r="23" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="103"/>
+      <c r="A23" s="93"/>
       <c r="C23" s="50"/>
       <c r="N23" s="56"/>
     </row>
     <row r="24" spans="1:14" s="45" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="103"/>
+      <c r="A24" s="93"/>
       <c r="C24" s="17"/>
       <c r="E24" s="37"/>
       <c r="F24" s="17"/>
-      <c r="I24" s="76" t="s">
+      <c r="I24" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="J24" s="86" t="s">
+      <c r="J24" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="K24" s="76" t="s">
+      <c r="K24" s="71" t="s">
         <v>20</v>
       </c>
       <c r="N24" s="56"/>
     </row>
     <row r="25" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="103"/>
+      <c r="A25" s="93"/>
       <c r="D25" s="37"/>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
-      <c r="I25" s="45" t="s">
+      <c r="I25" s="119" t="s">
         <v>21</v>
       </c>
+      <c r="J25" s="119"/>
+      <c r="K25" s="119"/>
+      <c r="L25" s="119"/>
       <c r="N25" s="56"/>
     </row>
     <row r="26" spans="1:14" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A26" s="103"/>
-      <c r="B26" s="62"/>
-      <c r="C26" s="75" t="s">
+      <c r="A26" s="93"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="75" t="s">
+      <c r="D26" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="79" t="s">
+      <c r="E26" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="75" t="s">
+      <c r="F26" s="70" t="s">
         <v>10</v>
       </c>
       <c r="I26" s="124" t="s">
@@ -30829,225 +30874,227 @@
       <c r="N26" s="56"/>
     </row>
     <row r="27" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="103"/>
-      <c r="B27" s="108" t="s">
+      <c r="A27" s="93"/>
+      <c r="B27" s="111" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="76" t="s">
+      <c r="C27" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="D27" s="77" t="s">
+      <c r="D27" s="105" t="s">
         <v>87</v>
       </c>
-      <c r="E27" s="78" t="s">
+      <c r="E27" s="106" t="s">
         <v>88</v>
       </c>
-      <c r="F27" s="77" t="s">
+      <c r="F27" s="72" t="s">
         <v>89</v>
       </c>
       <c r="I27" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="J27" s="107" t="s">
+      <c r="J27" s="108" t="s">
         <v>26</v>
       </c>
-      <c r="K27" s="107" t="s">
+      <c r="K27" s="108" t="s">
         <v>27</v>
       </c>
-      <c r="L27" s="107" t="s">
+      <c r="L27" s="108" t="s">
         <v>28</v>
       </c>
       <c r="N27" s="56"/>
     </row>
     <row r="28" spans="1:14" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="103"/>
-      <c r="B28" s="114"/>
-      <c r="C28" s="96" t="s">
+      <c r="A28" s="93"/>
+      <c r="B28" s="117"/>
+      <c r="C28" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="77" t="s">
+      <c r="D28" s="105" t="s">
         <v>90</v>
       </c>
-      <c r="E28" s="78" t="s">
+      <c r="E28" s="106" t="s">
         <v>91</v>
       </c>
-      <c r="F28" s="77" t="s">
+      <c r="F28" s="72" t="s">
         <v>92</v>
       </c>
       <c r="G28" s="50"/>
       <c r="I28" s="24"/>
-      <c r="J28" s="108"/>
-      <c r="K28" s="108"/>
-      <c r="L28" s="108"/>
+      <c r="J28" s="111"/>
+      <c r="K28" s="111"/>
+      <c r="L28" s="111"/>
       <c r="N28" s="56"/>
     </row>
     <row r="29" spans="1:14" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="103"/>
-      <c r="B29" s="114"/>
-      <c r="C29" s="96" t="s">
+      <c r="A29" s="93"/>
+      <c r="B29" s="117"/>
+      <c r="C29" s="89" t="s">
         <v>81</v>
       </c>
-      <c r="D29" s="97" t="s">
+      <c r="D29" s="105" t="s">
         <v>93</v>
       </c>
-      <c r="E29" s="98" t="s">
+      <c r="E29" s="106" t="s">
         <v>94</v>
       </c>
-      <c r="F29" s="97" t="s">
+      <c r="F29" s="72" t="s">
         <v>95</v>
       </c>
       <c r="G29" s="51"/>
-      <c r="I29" s="84" t="s">
+      <c r="I29" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="J29" s="87" t="s">
+      <c r="J29" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="K29" s="81"/>
-      <c r="L29" s="88" t="s">
+      <c r="K29" s="76"/>
+      <c r="L29" s="82" t="s">
         <v>51</v>
       </c>
       <c r="N29" s="57"/>
     </row>
     <row r="30" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="103"/>
-      <c r="B30" s="114"/>
-      <c r="C30" s="76" t="s">
+      <c r="A30" s="93"/>
+      <c r="B30" s="117"/>
+      <c r="C30" s="71" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="77" t="s">
+      <c r="D30" s="105" t="s">
         <v>96</v>
       </c>
-      <c r="E30" s="78" t="s">
+      <c r="E30" s="106" t="s">
         <v>97</v>
       </c>
-      <c r="F30" s="77" t="s">
+      <c r="F30" s="72" t="s">
         <v>98</v>
       </c>
-      <c r="I30" s="68"/>
-      <c r="J30" s="69"/>
-      <c r="K30" s="70"/>
-      <c r="L30" s="69"/>
+      <c r="I30" s="63"/>
+      <c r="J30" s="64"/>
+      <c r="K30" s="65"/>
+      <c r="L30" s="64"/>
       <c r="N30" s="56"/>
     </row>
     <row r="31" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="103"/>
-      <c r="B31" s="114"/>
-      <c r="C31" s="96" t="s">
+      <c r="A31" s="93"/>
+      <c r="B31" s="117"/>
+      <c r="C31" s="89" t="s">
         <v>83</v>
       </c>
-      <c r="D31" s="77" t="s">
+      <c r="D31" s="105" t="s">
         <v>99</v>
       </c>
-      <c r="E31" s="78" t="s">
+      <c r="E31" s="106" t="s">
         <v>100</v>
       </c>
-      <c r="F31" s="77" t="s">
+      <c r="F31" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="I31" s="84" t="s">
+      <c r="I31" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="J31" s="87" t="s">
+      <c r="J31" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="K31" s="81"/>
-      <c r="L31" s="87" t="s">
+      <c r="K31" s="76"/>
+      <c r="L31" s="81" t="s">
         <v>65</v>
       </c>
       <c r="N31" s="56"/>
     </row>
     <row r="32" spans="1:14" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="103"/>
-      <c r="B32" s="115"/>
-      <c r="C32" s="96" t="s">
+      <c r="A32" s="93"/>
+      <c r="B32" s="118"/>
+      <c r="C32" s="97" t="s">
         <v>72</v>
       </c>
-      <c r="D32" s="77" t="s">
+      <c r="D32" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="E32" s="78" t="s">
+      <c r="E32" s="96" t="s">
         <v>103</v>
       </c>
-      <c r="F32" s="77" t="s">
+      <c r="F32" s="95" t="s">
         <v>104</v>
       </c>
-      <c r="I32" s="68"/>
-      <c r="J32" s="71"/>
-      <c r="K32" s="69"/>
-      <c r="L32" s="72"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="66"/>
+      <c r="K32" s="64"/>
+      <c r="L32" s="67"/>
       <c r="N32" s="56"/>
     </row>
     <row r="33" spans="1:14" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="103"/>
-      <c r="I33" s="84" t="s">
+      <c r="A33" s="93"/>
+      <c r="B33" s="23"/>
+      <c r="I33" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="J33" s="87" t="s">
+      <c r="J33" s="81" t="s">
         <v>46</v>
       </c>
-      <c r="K33" s="81"/>
-      <c r="L33" s="87" t="s">
+      <c r="K33" s="76"/>
+      <c r="L33" s="81" t="s">
         <v>64</v>
       </c>
       <c r="N33" s="56"/>
     </row>
     <row r="34" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="103"/>
-      <c r="B34" s="108" t="s">
+      <c r="A34" s="93"/>
+      <c r="B34" s="111" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="76" t="s">
+      <c r="C34" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="77" t="s">
+      <c r="D34" s="72" t="s">
         <v>105</v>
       </c>
-      <c r="E34" s="78" t="s">
+      <c r="E34" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="F34" s="77" t="s">
+      <c r="F34" s="72" t="s">
         <v>107</v>
       </c>
       <c r="H34" s="39"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="71"/>
-      <c r="K34" s="71"/>
-      <c r="L34" s="74"/>
+      <c r="I34" s="68"/>
+      <c r="J34" s="66"/>
+      <c r="K34" s="66"/>
+      <c r="L34" s="69"/>
       <c r="N34" s="56"/>
     </row>
     <row r="35" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="103"/>
-      <c r="B35" s="115"/>
-      <c r="C35" s="95" t="s">
+      <c r="A35" s="93"/>
+      <c r="B35" s="118"/>
+      <c r="C35" s="98" t="s">
         <v>72</v>
       </c>
-      <c r="D35" s="77" t="s">
+      <c r="D35" s="95" t="s">
         <v>108</v>
       </c>
-      <c r="E35" s="78" t="s">
+      <c r="E35" s="96" t="s">
         <v>109</v>
       </c>
-      <c r="F35" s="77" t="s">
+      <c r="F35" s="95" t="s">
         <v>110</v>
       </c>
       <c r="G35" s="39"/>
       <c r="H35" s="39"/>
-      <c r="I35" s="84" t="s">
+      <c r="I35" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="J35" s="89"/>
-      <c r="K35" s="87" t="s">
+      <c r="J35" s="83"/>
+      <c r="K35" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="L35" s="90" t="s">
+      <c r="L35" s="84" t="s">
         <v>63</v>
       </c>
       <c r="M35" s="40"/>
       <c r="N35" s="56"/>
     </row>
     <row r="36" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="103"/>
+      <c r="A36" s="93"/>
+      <c r="B36" s="23"/>
       <c r="G36" s="39"/>
       <c r="H36" s="39"/>
       <c r="I36" s="39"/>
@@ -31058,70 +31105,70 @@
       <c r="N36" s="56"/>
     </row>
     <row r="37" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="103"/>
-      <c r="B37" s="108" t="s">
+      <c r="A37" s="93"/>
+      <c r="B37" s="111" t="s">
         <v>86</v>
       </c>
-      <c r="C37" s="76" t="s">
+      <c r="C37" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="77" t="s">
+      <c r="D37" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="E37" s="78" t="s">
+      <c r="E37" s="106" t="s">
         <v>74</v>
       </c>
-      <c r="F37" s="77" t="s">
+      <c r="F37" s="72" t="s">
         <v>75</v>
       </c>
       <c r="G37" s="39"/>
       <c r="H37" s="39"/>
-      <c r="I37" s="84" t="s">
+      <c r="I37" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="J37" s="109" t="s">
+      <c r="J37" s="112" t="s">
         <v>47</v>
       </c>
-      <c r="K37" s="110"/>
-      <c r="L37" s="111"/>
+      <c r="K37" s="113"/>
+      <c r="L37" s="114"/>
       <c r="M37" s="39"/>
       <c r="N37" s="56"/>
     </row>
     <row r="38" spans="1:14" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="103"/>
-      <c r="B38" s="115"/>
-      <c r="C38" s="95" t="s">
+      <c r="A38" s="93"/>
+      <c r="B38" s="118"/>
+      <c r="C38" s="98" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="77" t="s">
+      <c r="D38" s="95" t="s">
         <v>76</v>
       </c>
-      <c r="E38" s="78" t="s">
+      <c r="E38" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="F38" s="77" t="s">
+      <c r="F38" s="95" t="s">
         <v>78</v>
       </c>
       <c r="G38" s="41"/>
       <c r="H38" s="41"/>
-      <c r="I38" s="84" t="s">
+      <c r="I38" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="J38" s="109" t="s">
+      <c r="J38" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="K38" s="110"/>
-      <c r="L38" s="111"/>
+      <c r="K38" s="113"/>
+      <c r="L38" s="114"/>
       <c r="M38" s="40"/>
       <c r="N38" s="56"/>
     </row>
     <row r="39" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="103"/>
+      <c r="A39" s="93"/>
       <c r="M39" s="40"/>
       <c r="N39" s="56"/>
     </row>
     <row r="40" spans="1:14" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="103"/>
+      <c r="A40" s="93"/>
       <c r="B40" s="39"/>
       <c r="C40" s="39"/>
       <c r="D40" s="39"/>
@@ -31137,71 +31184,71 @@
       <c r="N40" s="56"/>
     </row>
     <row r="41" spans="1:14" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="103"/>
-      <c r="B41" s="112" t="s">
+      <c r="A41" s="93"/>
+      <c r="B41" s="115" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="112"/>
-      <c r="D41" s="112"/>
-      <c r="E41" s="112"/>
-      <c r="F41" s="112"/>
+      <c r="C41" s="115"/>
+      <c r="D41" s="115"/>
+      <c r="E41" s="115"/>
+      <c r="F41" s="115"/>
       <c r="G41" s="42"/>
       <c r="H41" s="39"/>
       <c r="M41" s="39"/>
       <c r="N41" s="56"/>
     </row>
     <row r="42" spans="1:14" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="103"/>
-      <c r="B42" s="140" t="s">
+      <c r="A42" s="93"/>
+      <c r="B42" s="130" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="140"/>
-      <c r="D42" s="140"/>
-      <c r="E42" s="140"/>
-      <c r="F42" s="140"/>
-      <c r="G42" s="140"/>
-      <c r="H42" s="140"/>
-      <c r="I42" s="140"/>
-      <c r="J42" s="140"/>
-      <c r="K42" s="140"/>
-      <c r="L42" s="140"/>
+      <c r="C42" s="130"/>
+      <c r="D42" s="130"/>
+      <c r="E42" s="130"/>
+      <c r="F42" s="130"/>
+      <c r="G42" s="130"/>
+      <c r="H42" s="130"/>
+      <c r="I42" s="130"/>
+      <c r="J42" s="130"/>
+      <c r="K42" s="130"/>
+      <c r="L42" s="130"/>
       <c r="M42" s="39"/>
       <c r="N42" s="58"/>
     </row>
     <row r="43" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A43" s="103"/>
-      <c r="B43" s="140"/>
-      <c r="C43" s="140"/>
-      <c r="D43" s="140"/>
-      <c r="E43" s="140"/>
-      <c r="F43" s="140"/>
-      <c r="G43" s="140"/>
-      <c r="H43" s="140"/>
-      <c r="I43" s="140"/>
-      <c r="J43" s="140"/>
-      <c r="K43" s="140"/>
-      <c r="L43" s="140"/>
+      <c r="A43" s="93"/>
+      <c r="B43" s="130"/>
+      <c r="C43" s="130"/>
+      <c r="D43" s="130"/>
+      <c r="E43" s="130"/>
+      <c r="F43" s="130"/>
+      <c r="G43" s="130"/>
+      <c r="H43" s="130"/>
+      <c r="I43" s="130"/>
+      <c r="J43" s="130"/>
+      <c r="K43" s="130"/>
+      <c r="L43" s="130"/>
       <c r="M43" s="39"/>
       <c r="N43" s="58"/>
     </row>
     <row r="44" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A44" s="103"/>
-      <c r="B44" s="140"/>
-      <c r="C44" s="140"/>
-      <c r="D44" s="140"/>
-      <c r="E44" s="140"/>
-      <c r="F44" s="140"/>
-      <c r="G44" s="140"/>
-      <c r="H44" s="140"/>
-      <c r="I44" s="140"/>
-      <c r="J44" s="140"/>
-      <c r="K44" s="140"/>
-      <c r="L44" s="140"/>
+      <c r="A44" s="93"/>
+      <c r="B44" s="130"/>
+      <c r="C44" s="130"/>
+      <c r="D44" s="130"/>
+      <c r="E44" s="130"/>
+      <c r="F44" s="130"/>
+      <c r="G44" s="130"/>
+      <c r="H44" s="130"/>
+      <c r="I44" s="130"/>
+      <c r="J44" s="130"/>
+      <c r="K44" s="130"/>
+      <c r="L44" s="130"/>
       <c r="M44" s="39"/>
       <c r="N44" s="58"/>
     </row>
     <row r="45" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="103"/>
+      <c r="A45" s="93"/>
       <c r="B45" s="44"/>
       <c r="C45" s="39"/>
       <c r="D45" s="39"/>
@@ -31213,7 +31260,7 @@
       <c r="N45" s="58"/>
     </row>
     <row r="46" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A46" s="103"/>
+      <c r="A46" s="93"/>
       <c r="B46" s="44"/>
       <c r="C46" s="39"/>
       <c r="D46" s="39"/>
@@ -31228,7 +31275,7 @@
       <c r="N46" s="58"/>
     </row>
     <row r="47" spans="1:14" s="45" customFormat="1" ht="76.349999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="103"/>
+      <c r="A47" s="93"/>
       <c r="B47" s="43"/>
       <c r="C47" s="39"/>
       <c r="D47" s="39"/>
@@ -31236,51 +31283,51 @@
       <c r="F47" s="39"/>
       <c r="G47" s="39"/>
       <c r="H47" s="39"/>
-      <c r="I47" s="73"/>
-      <c r="J47" s="71"/>
-      <c r="K47" s="71"/>
-      <c r="L47" s="74"/>
+      <c r="I47" s="68"/>
+      <c r="J47" s="66"/>
+      <c r="K47" s="66"/>
+      <c r="L47" s="69"/>
       <c r="M47" s="59"/>
       <c r="N47" s="58"/>
     </row>
     <row r="48" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A48" s="103"/>
+      <c r="A48" s="93"/>
       <c r="B48" s="43"/>
       <c r="C48" s="54"/>
       <c r="D48" s="17"/>
       <c r="E48" s="17"/>
       <c r="F48" s="55"/>
       <c r="G48" s="55"/>
-      <c r="H48" s="93"/>
-      <c r="I48" s="92"/>
-      <c r="J48" s="94"/>
-      <c r="K48" s="91"/>
-      <c r="L48" s="74"/>
+      <c r="H48" s="87"/>
+      <c r="I48" s="86"/>
+      <c r="J48" s="88"/>
+      <c r="K48" s="85"/>
+      <c r="L48" s="69"/>
       <c r="M48" s="59"/>
       <c r="N48" s="58"/>
     </row>
     <row r="49" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="100"/>
+      <c r="A49" s="90"/>
       <c r="B49" s="13"/>
-      <c r="C49" s="105" t="s">
+      <c r="C49" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="D49" s="106"/>
-      <c r="E49" s="106"/>
+      <c r="D49" s="110"/>
+      <c r="E49" s="110"/>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
-      <c r="H49" s="113" t="s">
+      <c r="H49" s="116" t="s">
         <v>36</v>
       </c>
-      <c r="I49" s="113"/>
-      <c r="J49" s="113"/>
+      <c r="I49" s="116"/>
+      <c r="J49" s="116"/>
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
       <c r="M49" s="12"/>
       <c r="N49" s="11"/>
     </row>
     <row r="50" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="104"/>
+      <c r="A50" s="94"/>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
@@ -31296,7 +31343,7 @@
       <c r="N50" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="34">
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="B42:L44"/>
     <mergeCell ref="A1:C5"/>
@@ -31307,7 +31354,6 @@
     <mergeCell ref="D1:J5"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="G16:G17"/>
-    <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="E16:E17"/>
@@ -31319,6 +31365,7 @@
     <mergeCell ref="I26:L26"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="M5:N5"/>
+    <mergeCell ref="B16:B18"/>
     <mergeCell ref="C49:E49"/>
     <mergeCell ref="J27:J28"/>
     <mergeCell ref="K27:K28"/>
@@ -31330,6 +31377,7 @@
     <mergeCell ref="B27:B32"/>
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="B37:B38"/>
+    <mergeCell ref="I25:L25"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
correciones de reportes diarios
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaBalanceEnergia.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaBalanceEnergia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SP\UNNA-App\AppOperacionalReporte\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\diario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91066975-D84F-41B1-BC16-CF135BBF1683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0006DD-DCA2-4C40-A212-401C22ECE3BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="445" xr2:uid="{9E40B278-673A-417E-9A41-08ACE2830EAA}"/>
   </bookViews>
@@ -1202,8 +1202,83 @@
     <xf numFmtId="10" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="18" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="18" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1237,81 +1312,6 @@
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="18" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="18" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -30388,8 +30388,8 @@
   </sheetPr>
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="130" zoomScaleNormal="70" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A21" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -30411,101 +30411,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="131"/>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="134" t="s">
+      <c r="A1" s="112"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="116" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
-      <c r="J1" s="134"/>
-      <c r="K1" s="127" t="s">
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="116"/>
+      <c r="K1" s="108" t="s">
         <v>67</v>
       </c>
-      <c r="L1" s="128"/>
-      <c r="M1" s="128"/>
-      <c r="N1" s="129"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="109"/>
+      <c r="N1" s="110"/>
     </row>
     <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="131"/>
-      <c r="B2" s="131"/>
-      <c r="C2" s="131"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="143" t="s">
+      <c r="A2" s="112"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="122"/>
-      <c r="M2" s="122"/>
-      <c r="N2" s="123"/>
+      <c r="L2" s="126"/>
+      <c r="M2" s="126"/>
+      <c r="N2" s="127"/>
     </row>
     <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="131"/>
-      <c r="B3" s="131"/>
-      <c r="C3" s="131"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-      <c r="H3" s="134"/>
-      <c r="I3" s="134"/>
-      <c r="J3" s="134"/>
-      <c r="K3" s="125" t="s">
+      <c r="A3" s="112"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="116"/>
+      <c r="F3" s="116"/>
+      <c r="G3" s="116"/>
+      <c r="H3" s="116"/>
+      <c r="I3" s="116"/>
+      <c r="J3" s="116"/>
+      <c r="K3" s="128" t="s">
         <v>68</v>
       </c>
-      <c r="L3" s="144"/>
-      <c r="M3" s="144"/>
-      <c r="N3" s="126"/>
+      <c r="L3" s="129"/>
+      <c r="M3" s="129"/>
+      <c r="N3" s="130"/>
     </row>
     <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="131"/>
-      <c r="B4" s="131"/>
-      <c r="C4" s="131"/>
-      <c r="D4" s="134"/>
-      <c r="E4" s="134"/>
-      <c r="F4" s="134"/>
-      <c r="G4" s="134"/>
-      <c r="H4" s="134"/>
-      <c r="I4" s="134"/>
-      <c r="J4" s="134"/>
-      <c r="K4" s="120" t="s">
+      <c r="A4" s="112"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
+      <c r="F4" s="116"/>
+      <c r="G4" s="116"/>
+      <c r="H4" s="116"/>
+      <c r="I4" s="116"/>
+      <c r="J4" s="116"/>
+      <c r="K4" s="131" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="121"/>
-      <c r="M4" s="122" t="s">
+      <c r="L4" s="132"/>
+      <c r="M4" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="123"/>
+      <c r="N4" s="127"/>
       <c r="O4" s="90"/>
     </row>
     <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="131"/>
-      <c r="B5" s="131"/>
-      <c r="C5" s="131"/>
-      <c r="D5" s="134"/>
-      <c r="E5" s="134"/>
-      <c r="F5" s="134"/>
-      <c r="G5" s="134"/>
-      <c r="H5" s="134"/>
-      <c r="I5" s="134"/>
-      <c r="J5" s="134"/>
-      <c r="K5" s="122" t="s">
+      <c r="A5" s="112"/>
+      <c r="B5" s="112"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="116"/>
+      <c r="E5" s="116"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="116"/>
+      <c r="H5" s="116"/>
+      <c r="I5" s="116"/>
+      <c r="J5" s="116"/>
+      <c r="K5" s="126" t="s">
         <v>69</v>
       </c>
-      <c r="L5" s="122"/>
-      <c r="M5" s="125" t="s">
+      <c r="L5" s="126"/>
+      <c r="M5" s="128" t="s">
         <v>70</v>
       </c>
-      <c r="N5" s="126"/>
+      <c r="N5" s="130"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="92"/>
@@ -30632,19 +30632,19 @@
     <row r="14" spans="1:15" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="93"/>
       <c r="B14" s="24"/>
-      <c r="C14" s="132" t="s">
+      <c r="C14" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="108" t="s">
+      <c r="D14" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="133" t="s">
+      <c r="E14" s="115" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="108" t="s">
+      <c r="F14" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="108" t="s">
+      <c r="G14" s="114" t="s">
         <v>11</v>
       </c>
       <c r="H14" s="25"/>
@@ -30660,11 +30660,11 @@
     <row r="15" spans="1:15" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="93"/>
       <c r="B15" s="24"/>
-      <c r="C15" s="132"/>
-      <c r="D15" s="108"/>
-      <c r="E15" s="133"/>
-      <c r="F15" s="108"/>
-      <c r="G15" s="108"/>
+      <c r="C15" s="113"/>
+      <c r="D15" s="114"/>
+      <c r="E15" s="115"/>
+      <c r="F15" s="114"/>
+      <c r="G15" s="114"/>
       <c r="H15" s="17"/>
       <c r="I15" s="77" t="s">
         <v>52</v>
@@ -30680,22 +30680,22 @@
     </row>
     <row r="16" spans="1:15" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="93"/>
-      <c r="B16" s="108" t="s">
+      <c r="B16" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="135" t="s">
+      <c r="C16" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="137" t="s">
+      <c r="D16" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="139" t="s">
+      <c r="E16" s="117" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="141" t="s">
+      <c r="F16" s="123" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="139" t="s">
+      <c r="G16" s="117" t="s">
         <v>41</v>
       </c>
       <c r="H16" s="17"/>
@@ -30714,12 +30714,12 @@
     </row>
     <row r="17" spans="1:14" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="93"/>
-      <c r="B17" s="108"/>
-      <c r="C17" s="136"/>
-      <c r="D17" s="138"/>
-      <c r="E17" s="140"/>
-      <c r="F17" s="142"/>
-      <c r="G17" s="140"/>
+      <c r="B17" s="114"/>
+      <c r="C17" s="120"/>
+      <c r="D17" s="122"/>
+      <c r="E17" s="118"/>
+      <c r="F17" s="124"/>
+      <c r="G17" s="118"/>
       <c r="H17" s="17"/>
       <c r="I17" s="77" t="s">
         <v>54</v>
@@ -30736,7 +30736,7 @@
     </row>
     <row r="18" spans="1:14" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="93"/>
-      <c r="B18" s="108"/>
+      <c r="B18" s="114"/>
       <c r="C18" s="99" t="s">
         <v>72</v>
       </c>
@@ -30842,12 +30842,12 @@
       <c r="D25" s="37"/>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
-      <c r="I25" s="119" t="s">
+      <c r="I25" s="144" t="s">
         <v>21</v>
       </c>
-      <c r="J25" s="119"/>
-      <c r="K25" s="119"/>
-      <c r="L25" s="119"/>
+      <c r="J25" s="144"/>
+      <c r="K25" s="144"/>
+      <c r="L25" s="144"/>
       <c r="N25" s="56"/>
     </row>
     <row r="26" spans="1:14" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -30865,17 +30865,17 @@
       <c r="F26" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="I26" s="124" t="s">
+      <c r="I26" s="133" t="s">
         <v>24</v>
       </c>
-      <c r="J26" s="124"/>
-      <c r="K26" s="124"/>
-      <c r="L26" s="124"/>
+      <c r="J26" s="133"/>
+      <c r="K26" s="133"/>
+      <c r="L26" s="133"/>
       <c r="N26" s="56"/>
     </row>
     <row r="27" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="93"/>
-      <c r="B27" s="111" t="s">
+      <c r="B27" s="136" t="s">
         <v>84</v>
       </c>
       <c r="C27" s="71" t="s">
@@ -30893,20 +30893,20 @@
       <c r="I27" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="J27" s="108" t="s">
+      <c r="J27" s="114" t="s">
         <v>26</v>
       </c>
-      <c r="K27" s="108" t="s">
+      <c r="K27" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="L27" s="108" t="s">
+      <c r="L27" s="114" t="s">
         <v>28</v>
       </c>
       <c r="N27" s="56"/>
     </row>
     <row r="28" spans="1:14" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="93"/>
-      <c r="B28" s="117"/>
+      <c r="B28" s="142"/>
       <c r="C28" s="89" t="s">
         <v>80</v>
       </c>
@@ -30921,14 +30921,14 @@
       </c>
       <c r="G28" s="50"/>
       <c r="I28" s="24"/>
-      <c r="J28" s="111"/>
-      <c r="K28" s="111"/>
-      <c r="L28" s="111"/>
+      <c r="J28" s="136"/>
+      <c r="K28" s="136"/>
+      <c r="L28" s="136"/>
       <c r="N28" s="56"/>
     </row>
     <row r="29" spans="1:14" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="93"/>
-      <c r="B29" s="117"/>
+      <c r="B29" s="142"/>
       <c r="C29" s="89" t="s">
         <v>81</v>
       </c>
@@ -30956,7 +30956,7 @@
     </row>
     <row r="30" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="93"/>
-      <c r="B30" s="117"/>
+      <c r="B30" s="142"/>
       <c r="C30" s="71" t="s">
         <v>82</v>
       </c>
@@ -30977,7 +30977,7 @@
     </row>
     <row r="31" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="93"/>
-      <c r="B31" s="117"/>
+      <c r="B31" s="142"/>
       <c r="C31" s="89" t="s">
         <v>83</v>
       </c>
@@ -31004,7 +31004,7 @@
     </row>
     <row r="32" spans="1:14" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="93"/>
-      <c r="B32" s="118"/>
+      <c r="B32" s="143"/>
       <c r="C32" s="97" t="s">
         <v>72</v>
       </c>
@@ -31040,7 +31040,7 @@
     </row>
     <row r="34" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="93"/>
-      <c r="B34" s="111" t="s">
+      <c r="B34" s="136" t="s">
         <v>85</v>
       </c>
       <c r="C34" s="71" t="s">
@@ -31064,7 +31064,7 @@
     </row>
     <row r="35" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="93"/>
-      <c r="B35" s="118"/>
+      <c r="B35" s="143"/>
       <c r="C35" s="98" t="s">
         <v>72</v>
       </c>
@@ -31106,7 +31106,7 @@
     </row>
     <row r="37" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="93"/>
-      <c r="B37" s="111" t="s">
+      <c r="B37" s="136" t="s">
         <v>86</v>
       </c>
       <c r="C37" s="71" t="s">
@@ -31126,17 +31126,17 @@
       <c r="I37" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="J37" s="112" t="s">
+      <c r="J37" s="137" t="s">
         <v>47</v>
       </c>
-      <c r="K37" s="113"/>
-      <c r="L37" s="114"/>
+      <c r="K37" s="138"/>
+      <c r="L37" s="139"/>
       <c r="M37" s="39"/>
       <c r="N37" s="56"/>
     </row>
     <row r="38" spans="1:14" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A38" s="93"/>
-      <c r="B38" s="118"/>
+      <c r="B38" s="143"/>
       <c r="C38" s="98" t="s">
         <v>72</v>
       </c>
@@ -31154,11 +31154,11 @@
       <c r="I38" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="J38" s="112" t="s">
+      <c r="J38" s="137" t="s">
         <v>48</v>
       </c>
-      <c r="K38" s="113"/>
-      <c r="L38" s="114"/>
+      <c r="K38" s="138"/>
+      <c r="L38" s="139"/>
       <c r="M38" s="40"/>
       <c r="N38" s="56"/>
     </row>
@@ -31169,11 +31169,13 @@
     </row>
     <row r="40" spans="1:14" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="93"/>
-      <c r="B40" s="39"/>
-      <c r="C40" s="39"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="39"/>
-      <c r="F40" s="39"/>
+      <c r="B40" s="140" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="140"/>
+      <c r="D40" s="140"/>
+      <c r="E40" s="140"/>
+      <c r="F40" s="140"/>
       <c r="G40" s="42"/>
       <c r="H40" s="39"/>
       <c r="I40" s="18"/>
@@ -31185,77 +31187,83 @@
     </row>
     <row r="41" spans="1:14" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="93"/>
-      <c r="B41" s="115" t="s">
-        <v>35</v>
+      <c r="B41" s="111" t="s">
+        <v>49</v>
       </c>
-      <c r="C41" s="115"/>
-      <c r="D41" s="115"/>
-      <c r="E41" s="115"/>
-      <c r="F41" s="115"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="39"/>
+      <c r="C41" s="111"/>
+      <c r="D41" s="111"/>
+      <c r="E41" s="111"/>
+      <c r="F41" s="111"/>
+      <c r="G41" s="111"/>
+      <c r="H41" s="111"/>
+      <c r="I41" s="111"/>
+      <c r="J41" s="111"/>
+      <c r="K41" s="111"/>
+      <c r="L41" s="111"/>
       <c r="M41" s="39"/>
       <c r="N41" s="56"/>
     </row>
     <row r="42" spans="1:14" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="93"/>
-      <c r="B42" s="130" t="s">
-        <v>49</v>
-      </c>
-      <c r="C42" s="130"/>
-      <c r="D42" s="130"/>
-      <c r="E42" s="130"/>
-      <c r="F42" s="130"/>
-      <c r="G42" s="130"/>
-      <c r="H42" s="130"/>
-      <c r="I42" s="130"/>
-      <c r="J42" s="130"/>
-      <c r="K42" s="130"/>
-      <c r="L42" s="130"/>
+      <c r="B42" s="111"/>
+      <c r="C42" s="111"/>
+      <c r="D42" s="111"/>
+      <c r="E42" s="111"/>
+      <c r="F42" s="111"/>
+      <c r="G42" s="111"/>
+      <c r="H42" s="111"/>
+      <c r="I42" s="111"/>
+      <c r="J42" s="111"/>
+      <c r="K42" s="111"/>
+      <c r="L42" s="111"/>
       <c r="M42" s="39"/>
       <c r="N42" s="58"/>
     </row>
     <row r="43" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="93"/>
-      <c r="B43" s="130"/>
-      <c r="C43" s="130"/>
-      <c r="D43" s="130"/>
-      <c r="E43" s="130"/>
-      <c r="F43" s="130"/>
-      <c r="G43" s="130"/>
-      <c r="H43" s="130"/>
-      <c r="I43" s="130"/>
-      <c r="J43" s="130"/>
-      <c r="K43" s="130"/>
-      <c r="L43" s="130"/>
+      <c r="B43" s="111"/>
+      <c r="C43" s="111"/>
+      <c r="D43" s="111"/>
+      <c r="E43" s="111"/>
+      <c r="F43" s="111"/>
+      <c r="G43" s="111"/>
+      <c r="H43" s="111"/>
+      <c r="I43" s="111"/>
+      <c r="J43" s="111"/>
+      <c r="K43" s="111"/>
+      <c r="L43" s="111"/>
       <c r="M43" s="39"/>
       <c r="N43" s="58"/>
     </row>
     <row r="44" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="93"/>
-      <c r="B44" s="130"/>
-      <c r="C44" s="130"/>
-      <c r="D44" s="130"/>
-      <c r="E44" s="130"/>
-      <c r="F44" s="130"/>
-      <c r="G44" s="130"/>
-      <c r="H44" s="130"/>
-      <c r="I44" s="130"/>
-      <c r="J44" s="130"/>
-      <c r="K44" s="130"/>
-      <c r="L44" s="130"/>
+      <c r="B44" s="111"/>
+      <c r="C44" s="111"/>
+      <c r="D44" s="111"/>
+      <c r="E44" s="111"/>
+      <c r="F44" s="111"/>
+      <c r="G44" s="111"/>
+      <c r="H44" s="111"/>
+      <c r="I44" s="111"/>
+      <c r="J44" s="111"/>
+      <c r="K44" s="111"/>
+      <c r="L44" s="111"/>
       <c r="M44" s="39"/>
       <c r="N44" s="58"/>
     </row>
     <row r="45" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="93"/>
-      <c r="B45" s="44"/>
-      <c r="C45" s="39"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="39"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
+      <c r="B45" s="111"/>
+      <c r="C45" s="111"/>
+      <c r="D45" s="111"/>
+      <c r="E45" s="111"/>
+      <c r="F45" s="111"/>
+      <c r="G45" s="111"/>
+      <c r="H45" s="111"/>
+      <c r="I45" s="111"/>
+      <c r="J45" s="111"/>
+      <c r="K45" s="111"/>
+      <c r="L45" s="111"/>
       <c r="M45" s="59"/>
       <c r="N45" s="58"/>
     </row>
@@ -31309,18 +31317,18 @@
     <row r="49" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="90"/>
       <c r="B49" s="13"/>
-      <c r="C49" s="109" t="s">
+      <c r="C49" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="D49" s="110"/>
-      <c r="E49" s="110"/>
+      <c r="D49" s="135"/>
+      <c r="E49" s="135"/>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
-      <c r="H49" s="116" t="s">
+      <c r="H49" s="141" t="s">
         <v>36</v>
       </c>
-      <c r="I49" s="116"/>
-      <c r="J49" s="116"/>
+      <c r="I49" s="141"/>
+      <c r="J49" s="141"/>
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
       <c r="M49" s="12"/>
@@ -31344,8 +31352,26 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="K27:K28"/>
+    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="H49:J49"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="I25:L25"/>
+    <mergeCell ref="B41:L45"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="I26:L26"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
     <mergeCell ref="K1:N1"/>
-    <mergeCell ref="B42:L44"/>
     <mergeCell ref="A1:C5"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
@@ -31360,24 +31386,6 @@
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="K3:N3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="I26:L26"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="J27:J28"/>
-    <mergeCell ref="K27:K28"/>
-    <mergeCell ref="L27:L28"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="H49:J49"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="I25:L25"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
actualizacion de diseño en BoletaBalanceEnergia
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaBalanceEnergia.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/diario/BoletaBalanceEnergia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27820"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SP\UNNA-App\AppOperacionalReporte\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\diario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza7\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\diario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0006DD-DCA2-4C40-A212-401C22ECE3BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6CA5E1-9C5D-42A8-8BC6-E622FB151837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="445" xr2:uid="{9E40B278-673A-417E-9A41-08ACE2830EAA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="445" xr2:uid="{9E40B278-673A-417E-9A41-08ACE2830EAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Boleta ENEL" sheetId="1" r:id="rId1"/>
@@ -560,9 +560,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-280A]dddd\ d&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -887,7 +888,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="138">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -937,348 +938,248 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="4" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="12" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="6" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="6" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="6" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="6" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="6" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="6" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="18" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="18" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="18" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="18" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="18" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1286,32 +1187,113 @@
     <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="9" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="9" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="10" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="11" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="18" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="18" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1453,7 +1435,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="BOL"/>
@@ -1494,7 +1476,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink10.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="MOLLENDO DIARIO"/>
@@ -1511,7 +1493,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Correción 4606B"/>
@@ -1586,7 +1568,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="ROMT"/>
@@ -22466,7 +22448,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="TABLAS"/>
@@ -23075,7 +23057,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="..."/>
@@ -23172,7 +23154,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="XXXXXXX"/>
@@ -28255,7 +28237,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="..."/>
@@ -28415,7 +28397,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Datos"/>
@@ -28440,7 +28422,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="FECHA"/>
@@ -28726,7 +28708,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="COMPRAS DE GAS"/>
@@ -30388,129 +30370,129 @@
   </sheetPr>
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A21" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A12" zoomScaleNormal="70" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16:G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.54296875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" style="1" customWidth="1"/>
-    <col min="6" max="7" width="10.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.21875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.90625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.08984375" style="1" customWidth="1"/>
+    <col min="6" max="7" width="10.81640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1796875" style="1" customWidth="1"/>
     <col min="9" max="9" width="30" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.77734375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.21875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="8.77734375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.77734375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="7.33203125" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.5546875" style="1"/>
+    <col min="10" max="10" width="10.81640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1796875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.81640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.81640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="7.36328125" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="112"/>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="116" t="s">
+    <row r="1" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A1" s="122"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="125" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116"/>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
-      <c r="J1" s="116"/>
-      <c r="K1" s="108" t="s">
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="119" t="s">
         <v>67</v>
       </c>
-      <c r="L1" s="109"/>
-      <c r="M1" s="109"/>
-      <c r="N1" s="110"/>
+      <c r="L1" s="120"/>
+      <c r="M1" s="120"/>
+      <c r="N1" s="121"/>
     </row>
-    <row r="2" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="112"/>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="125" t="s">
+    <row r="2" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A2" s="122"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="126"/>
-      <c r="M2" s="126"/>
-      <c r="N2" s="127"/>
+      <c r="L2" s="114"/>
+      <c r="M2" s="114"/>
+      <c r="N2" s="115"/>
     </row>
-    <row r="3" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="112"/>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="116"/>
-      <c r="H3" s="116"/>
-      <c r="I3" s="116"/>
-      <c r="J3" s="116"/>
-      <c r="K3" s="128" t="s">
+    <row r="3" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="122"/>
+      <c r="B3" s="122"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="125"/>
+      <c r="K3" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="L3" s="129"/>
-      <c r="M3" s="129"/>
-      <c r="N3" s="130"/>
+      <c r="L3" s="135"/>
+      <c r="M3" s="135"/>
+      <c r="N3" s="118"/>
     </row>
-    <row r="4" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="112"/>
-      <c r="B4" s="112"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="116"/>
-      <c r="E4" s="116"/>
-      <c r="F4" s="116"/>
-      <c r="G4" s="116"/>
-      <c r="H4" s="116"/>
-      <c r="I4" s="116"/>
-      <c r="J4" s="116"/>
-      <c r="K4" s="131" t="s">
+    <row r="4" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="122"/>
+      <c r="B4" s="122"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="125"/>
+      <c r="E4" s="125"/>
+      <c r="F4" s="125"/>
+      <c r="G4" s="125"/>
+      <c r="H4" s="125"/>
+      <c r="I4" s="125"/>
+      <c r="J4" s="125"/>
+      <c r="K4" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="132"/>
-      <c r="M4" s="126" t="s">
+      <c r="L4" s="113"/>
+      <c r="M4" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="127"/>
-      <c r="O4" s="90"/>
+      <c r="N4" s="115"/>
+      <c r="O4" s="84"/>
     </row>
-    <row r="5" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="112"/>
-      <c r="B5" s="112"/>
-      <c r="C5" s="112"/>
-      <c r="D5" s="116"/>
-      <c r="E5" s="116"/>
-      <c r="F5" s="116"/>
-      <c r="G5" s="116"/>
-      <c r="H5" s="116"/>
-      <c r="I5" s="116"/>
-      <c r="J5" s="116"/>
-      <c r="K5" s="126" t="s">
+    <row r="5" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="122"/>
+      <c r="B5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="125"/>
+      <c r="E5" s="125"/>
+      <c r="F5" s="125"/>
+      <c r="G5" s="125"/>
+      <c r="H5" s="125"/>
+      <c r="I5" s="125"/>
+      <c r="J5" s="125"/>
+      <c r="K5" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="L5" s="126"/>
-      <c r="M5" s="128" t="s">
+      <c r="L5" s="114"/>
+      <c r="M5" s="117" t="s">
         <v>70</v>
       </c>
-      <c r="N5" s="130"/>
+      <c r="N5" s="118"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="92"/>
-      <c r="B6" s="91"/>
-      <c r="C6" s="91"/>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="85"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -30523,8 +30505,8 @@
       <c r="M6" s="2"/>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:15" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="90"/>
+    <row r="7" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="84"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="5" t="s">
@@ -30541,8 +30523,8 @@
       <c r="M7" s="4"/>
       <c r="N7" s="7"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="90"/>
+    <row r="8" spans="1:15" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="84"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="6"/>
@@ -30559,8 +30541,8 @@
       <c r="M8" s="4"/>
       <c r="N8" s="7"/>
     </row>
-    <row r="9" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="90"/>
+    <row r="9" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="84"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="6"/>
@@ -30575,22 +30557,22 @@
       <c r="M9" s="4"/>
       <c r="N9" s="7"/>
     </row>
-    <row r="10" spans="1:15" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="93"/>
+    <row r="10" spans="1:15" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A10" s="84"/>
       <c r="B10" s="17"/>
       <c r="G10" s="18"/>
       <c r="H10" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="104" t="s">
+      <c r="I10" s="95" t="s">
         <v>50</v>
       </c>
       <c r="L10" s="21"/>
       <c r="M10" s="21"/>
-      <c r="N10" s="56"/>
+      <c r="N10" s="55"/>
     </row>
-    <row r="11" spans="1:15" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="93"/>
+    <row r="11" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="84"/>
       <c r="B11" s="19"/>
       <c r="C11" s="17"/>
       <c r="E11" s="17"/>
@@ -30602,10 +30584,10 @@
       <c r="K11" s="17"/>
       <c r="L11" s="21"/>
       <c r="M11" s="21"/>
-      <c r="N11" s="56"/>
+      <c r="N11" s="55"/>
     </row>
-    <row r="12" spans="1:15" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="93"/>
+    <row r="12" spans="1:15" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A12" s="84"/>
       <c r="B12" s="22"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -30616,10 +30598,10 @@
       <c r="I12" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="N12" s="56"/>
+      <c r="N12" s="55"/>
     </row>
-    <row r="13" spans="1:15" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="93"/>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="84"/>
       <c r="B13" s="23"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -30627,141 +30609,141 @@
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
       <c r="H13" s="17"/>
-      <c r="N13" s="56"/>
+      <c r="N13" s="55"/>
     </row>
-    <row r="14" spans="1:15" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A14" s="93"/>
+    <row r="14" spans="1:15" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A14" s="84"/>
       <c r="B14" s="24"/>
-      <c r="C14" s="113" t="s">
+      <c r="C14" s="123" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="114" t="s">
+      <c r="D14" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="115" t="s">
+      <c r="E14" s="124" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="114" t="s">
+      <c r="F14" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="114" t="s">
+      <c r="G14" s="99" t="s">
         <v>11</v>
       </c>
       <c r="H14" s="25"/>
       <c r="I14" s="24"/>
-      <c r="J14" s="75" t="s">
+      <c r="J14" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="K14" s="75" t="s">
+      <c r="K14" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="N14" s="56"/>
+      <c r="N14" s="55"/>
     </row>
-    <row r="15" spans="1:15" s="45" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="93"/>
+    <row r="15" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="84"/>
       <c r="B15" s="24"/>
-      <c r="C15" s="113"/>
-      <c r="D15" s="114"/>
-      <c r="E15" s="115"/>
-      <c r="F15" s="114"/>
-      <c r="G15" s="114"/>
+      <c r="C15" s="123"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="99"/>
+      <c r="G15" s="99"/>
       <c r="H15" s="17"/>
-      <c r="I15" s="77" t="s">
+      <c r="I15" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="J15" s="103" t="s">
+      <c r="J15" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="K15" s="103" t="s">
+      <c r="K15" s="94" t="s">
         <v>56</v>
       </c>
-      <c r="L15" s="46"/>
-      <c r="N15" s="56"/>
+      <c r="L15" s="45"/>
+      <c r="N15" s="55"/>
     </row>
-    <row r="16" spans="1:15" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="93"/>
-      <c r="B16" s="114" t="s">
+    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="84"/>
+      <c r="B16" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="119" t="s">
+      <c r="C16" s="128" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="121" t="s">
+      <c r="D16" s="130" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="117" t="s">
+      <c r="E16" s="126" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="123" t="s">
+      <c r="F16" s="132" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="117" t="s">
+      <c r="G16" s="136" t="s">
         <v>41</v>
       </c>
       <c r="H16" s="17"/>
-      <c r="I16" s="77" t="s">
+      <c r="I16" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="J16" s="103" t="s">
+      <c r="J16" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="K16" s="103" t="s">
+      <c r="K16" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="L16" s="47"/>
+      <c r="L16" s="46"/>
       <c r="M16" s="37"/>
-      <c r="N16" s="56"/>
+      <c r="N16" s="55"/>
     </row>
-    <row r="17" spans="1:14" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="93"/>
-      <c r="B17" s="114"/>
-      <c r="C17" s="120"/>
-      <c r="D17" s="122"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="124"/>
-      <c r="G17" s="118"/>
+    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="84"/>
+      <c r="B17" s="99"/>
+      <c r="C17" s="129"/>
+      <c r="D17" s="131"/>
+      <c r="E17" s="127"/>
+      <c r="F17" s="133"/>
+      <c r="G17" s="137"/>
       <c r="H17" s="17"/>
-      <c r="I17" s="77" t="s">
+      <c r="I17" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="J17" s="103" t="s">
+      <c r="J17" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="K17" s="103" t="s">
+      <c r="K17" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="L17" s="47"/>
+      <c r="L17" s="46"/>
       <c r="M17" s="37"/>
-      <c r="N17" s="56"/>
+      <c r="N17" s="55"/>
     </row>
-    <row r="18" spans="1:14" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="93"/>
-      <c r="B18" s="114"/>
-      <c r="C18" s="99" t="s">
+    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="84"/>
+      <c r="B18" s="99"/>
+      <c r="C18" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="100" t="s">
+      <c r="D18" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="101" t="s">
+      <c r="E18" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="100" t="s">
+      <c r="F18" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="102" t="s">
+      <c r="G18" s="93" t="s">
         <v>41</v>
       </c>
       <c r="H18" s="17"/>
-      <c r="I18" s="61"/>
-      <c r="J18" s="62"/>
-      <c r="K18" s="62"/>
-      <c r="L18" s="47"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="46"/>
       <c r="M18" s="37"/>
-      <c r="N18" s="56"/>
+      <c r="N18" s="55"/>
     </row>
-    <row r="19" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="93"/>
+    <row r="19" spans="1:14" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A19" s="84"/>
       <c r="B19" s="26"/>
       <c r="C19" s="27"/>
       <c r="D19" s="28"/>
@@ -30772,18 +30754,18 @@
       <c r="I19" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="L19" s="48"/>
-      <c r="N19" s="56"/>
+      <c r="L19" s="47"/>
+      <c r="N19" s="55"/>
     </row>
-    <row r="20" spans="1:14" s="45" customFormat="1" ht="25.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="93"/>
+    <row r="20" spans="1:14" ht="25.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="84"/>
       <c r="B20" s="32"/>
       <c r="H20" s="33"/>
-      <c r="L20" s="48"/>
-      <c r="N20" s="56"/>
+      <c r="L20" s="47"/>
+      <c r="N20" s="55"/>
     </row>
-    <row r="21" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="93"/>
+    <row r="21" spans="1:14" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A21" s="84"/>
       <c r="B21" s="34"/>
       <c r="C21" s="19"/>
       <c r="D21" s="35"/>
@@ -30791,391 +30773,391 @@
       <c r="F21" s="33"/>
       <c r="G21" s="33"/>
       <c r="H21" s="33"/>
-      <c r="I21" s="78" t="s">
+      <c r="I21" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="J21" s="79" t="s">
+      <c r="J21" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="K21" s="49"/>
-      <c r="L21" s="50"/>
-      <c r="N21" s="56"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="49"/>
+      <c r="N21" s="55"/>
     </row>
-    <row r="22" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="93"/>
+    <row r="22" spans="1:14" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A22" s="84"/>
       <c r="B22" s="36"/>
-      <c r="E22" s="45" t="s">
+      <c r="E22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I22" s="78" t="s">
+      <c r="I22" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="J22" s="107" t="s">
+      <c r="J22" s="98" t="s">
         <v>61</v>
       </c>
-      <c r="K22" s="48"/>
-      <c r="N22" s="56"/>
+      <c r="K22" s="47"/>
+      <c r="N22" s="55"/>
     </row>
-    <row r="23" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="93"/>
-      <c r="C23" s="50"/>
-      <c r="N23" s="56"/>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="84"/>
+      <c r="C23" s="49"/>
+      <c r="N23" s="55"/>
     </row>
-    <row r="24" spans="1:14" s="45" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="93"/>
+    <row r="24" spans="1:14" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A24" s="84"/>
       <c r="C24" s="17"/>
       <c r="E24" s="37"/>
       <c r="F24" s="17"/>
-      <c r="I24" s="71" t="s">
+      <c r="I24" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="J24" s="80" t="s">
+      <c r="J24" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="K24" s="71" t="s">
+      <c r="K24" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="N24" s="56"/>
+      <c r="N24" s="55"/>
     </row>
-    <row r="25" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="93"/>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="84"/>
       <c r="D25" s="37"/>
       <c r="E25" s="17"/>
       <c r="F25" s="17"/>
-      <c r="I25" s="144" t="s">
+      <c r="I25" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="J25" s="144"/>
-      <c r="K25" s="144"/>
-      <c r="L25" s="144"/>
-      <c r="N25" s="56"/>
+      <c r="J25" s="110"/>
+      <c r="K25" s="110"/>
+      <c r="L25" s="110"/>
+      <c r="N25" s="55"/>
     </row>
-    <row r="26" spans="1:14" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A26" s="93"/>
-      <c r="B26" s="60"/>
-      <c r="C26" s="70" t="s">
+    <row r="26" spans="1:14" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A26" s="84"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="70" t="s">
+      <c r="D26" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="74" t="s">
+      <c r="E26" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="70" t="s">
+      <c r="F26" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="I26" s="133" t="s">
+      <c r="I26" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="J26" s="133"/>
-      <c r="K26" s="133"/>
-      <c r="L26" s="133"/>
-      <c r="N26" s="56"/>
+      <c r="J26" s="116"/>
+      <c r="K26" s="116"/>
+      <c r="L26" s="116"/>
+      <c r="N26" s="55"/>
     </row>
-    <row r="27" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="93"/>
-      <c r="B27" s="136" t="s">
+    <row r="27" spans="1:14" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A27" s="84"/>
+      <c r="B27" s="102" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="71" t="s">
+      <c r="C27" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="D27" s="105" t="s">
+      <c r="D27" s="96" t="s">
         <v>87</v>
       </c>
-      <c r="E27" s="106" t="s">
+      <c r="E27" s="97" t="s">
         <v>88</v>
       </c>
-      <c r="F27" s="72" t="s">
+      <c r="F27" s="67" t="s">
         <v>89</v>
       </c>
       <c r="I27" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="J27" s="114" t="s">
+      <c r="J27" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="K27" s="114" t="s">
+      <c r="K27" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="L27" s="114" t="s">
+      <c r="L27" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="N27" s="56"/>
+      <c r="N27" s="55"/>
     </row>
-    <row r="28" spans="1:14" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="93"/>
-      <c r="B28" s="142"/>
-      <c r="C28" s="89" t="s">
+    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="84"/>
+      <c r="B28" s="108"/>
+      <c r="C28" s="83" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="105" t="s">
+      <c r="D28" s="96" t="s">
         <v>90</v>
       </c>
-      <c r="E28" s="106" t="s">
+      <c r="E28" s="97" t="s">
         <v>91</v>
       </c>
-      <c r="F28" s="72" t="s">
+      <c r="F28" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="G28" s="50"/>
+      <c r="G28" s="49"/>
       <c r="I28" s="24"/>
-      <c r="J28" s="136"/>
-      <c r="K28" s="136"/>
-      <c r="L28" s="136"/>
-      <c r="N28" s="56"/>
+      <c r="J28" s="102"/>
+      <c r="K28" s="102"/>
+      <c r="L28" s="102"/>
+      <c r="N28" s="55"/>
     </row>
-    <row r="29" spans="1:14" s="45" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="93"/>
-      <c r="B29" s="142"/>
-      <c r="C29" s="89" t="s">
+    <row r="29" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="84"/>
+      <c r="B29" s="108"/>
+      <c r="C29" s="83" t="s">
         <v>81</v>
       </c>
-      <c r="D29" s="105" t="s">
+      <c r="D29" s="96" t="s">
         <v>93</v>
       </c>
-      <c r="E29" s="106" t="s">
+      <c r="E29" s="97" t="s">
         <v>94</v>
       </c>
-      <c r="F29" s="72" t="s">
+      <c r="F29" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="G29" s="51"/>
-      <c r="I29" s="78" t="s">
+      <c r="G29" s="50"/>
+      <c r="I29" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="J29" s="81" t="s">
+      <c r="J29" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="K29" s="76"/>
-      <c r="L29" s="82" t="s">
+      <c r="K29" s="71"/>
+      <c r="L29" s="77" t="s">
         <v>51</v>
       </c>
-      <c r="N29" s="57"/>
+      <c r="N29" s="56"/>
     </row>
-    <row r="30" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="93"/>
-      <c r="B30" s="142"/>
-      <c r="C30" s="71" t="s">
+    <row r="30" spans="1:14" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A30" s="84"/>
+      <c r="B30" s="108"/>
+      <c r="C30" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="105" t="s">
+      <c r="D30" s="96" t="s">
         <v>96</v>
       </c>
-      <c r="E30" s="106" t="s">
+      <c r="E30" s="97" t="s">
         <v>97</v>
       </c>
-      <c r="F30" s="72" t="s">
+      <c r="F30" s="67" t="s">
         <v>98</v>
       </c>
-      <c r="I30" s="63"/>
-      <c r="J30" s="64"/>
-      <c r="K30" s="65"/>
-      <c r="L30" s="64"/>
-      <c r="N30" s="56"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="61"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="61"/>
+      <c r="N30" s="55"/>
     </row>
-    <row r="31" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="93"/>
-      <c r="B31" s="142"/>
-      <c r="C31" s="89" t="s">
+    <row r="31" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="84"/>
+      <c r="B31" s="108"/>
+      <c r="C31" s="83" t="s">
         <v>83</v>
       </c>
-      <c r="D31" s="105" t="s">
+      <c r="D31" s="96" t="s">
         <v>99</v>
       </c>
-      <c r="E31" s="106" t="s">
+      <c r="E31" s="97" t="s">
         <v>100</v>
       </c>
-      <c r="F31" s="72" t="s">
+      <c r="F31" s="67" t="s">
         <v>101</v>
       </c>
-      <c r="I31" s="78" t="s">
+      <c r="I31" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="J31" s="81" t="s">
+      <c r="J31" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="K31" s="76"/>
-      <c r="L31" s="81" t="s">
+      <c r="K31" s="71"/>
+      <c r="L31" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="N31" s="56"/>
+      <c r="N31" s="55"/>
     </row>
-    <row r="32" spans="1:14" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="93"/>
-      <c r="B32" s="143"/>
-      <c r="C32" s="97" t="s">
+    <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="84"/>
+      <c r="B32" s="109"/>
+      <c r="C32" s="83" t="s">
         <v>72</v>
       </c>
-      <c r="D32" s="95" t="s">
+      <c r="D32" s="87" t="s">
         <v>102</v>
       </c>
-      <c r="E32" s="96" t="s">
+      <c r="E32" s="88" t="s">
         <v>103</v>
       </c>
-      <c r="F32" s="95" t="s">
+      <c r="F32" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="I32" s="63"/>
-      <c r="J32" s="66"/>
-      <c r="K32" s="64"/>
-      <c r="L32" s="67"/>
-      <c r="N32" s="56"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="62"/>
+      <c r="K32" s="61"/>
+      <c r="L32" s="63"/>
+      <c r="N32" s="55"/>
     </row>
-    <row r="33" spans="1:14" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="93"/>
+    <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="84"/>
       <c r="B33" s="23"/>
-      <c r="I33" s="78" t="s">
+      <c r="I33" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="J33" s="81" t="s">
+      <c r="J33" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="K33" s="76"/>
-      <c r="L33" s="81" t="s">
+      <c r="K33" s="71"/>
+      <c r="L33" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="N33" s="56"/>
+      <c r="N33" s="55"/>
     </row>
-    <row r="34" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="93"/>
-      <c r="B34" s="136" t="s">
+    <row r="34" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="84"/>
+      <c r="B34" s="102" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="71" t="s">
+      <c r="C34" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="72" t="s">
+      <c r="D34" s="67" t="s">
         <v>105</v>
       </c>
-      <c r="E34" s="73" t="s">
+      <c r="E34" s="68" t="s">
         <v>106</v>
       </c>
-      <c r="F34" s="72" t="s">
+      <c r="F34" s="67" t="s">
         <v>107</v>
       </c>
       <c r="H34" s="39"/>
-      <c r="I34" s="68"/>
-      <c r="J34" s="66"/>
-      <c r="K34" s="66"/>
-      <c r="L34" s="69"/>
-      <c r="N34" s="56"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="62"/>
+      <c r="K34" s="62"/>
+      <c r="L34" s="64"/>
+      <c r="N34" s="55"/>
     </row>
-    <row r="35" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="93"/>
-      <c r="B35" s="143"/>
-      <c r="C35" s="98" t="s">
+    <row r="35" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="84"/>
+      <c r="B35" s="109"/>
+      <c r="C35" s="89" t="s">
         <v>72</v>
       </c>
-      <c r="D35" s="95" t="s">
+      <c r="D35" s="87" t="s">
         <v>108</v>
       </c>
-      <c r="E35" s="96" t="s">
+      <c r="E35" s="88" t="s">
         <v>109</v>
       </c>
-      <c r="F35" s="95" t="s">
+      <c r="F35" s="87" t="s">
         <v>110</v>
       </c>
       <c r="G35" s="39"/>
       <c r="H35" s="39"/>
-      <c r="I35" s="78" t="s">
+      <c r="I35" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="J35" s="83"/>
-      <c r="K35" s="81" t="s">
+      <c r="J35" s="78"/>
+      <c r="K35" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="L35" s="84" t="s">
+      <c r="L35" s="79" t="s">
         <v>63</v>
       </c>
       <c r="M35" s="40"/>
-      <c r="N35" s="56"/>
+      <c r="N35" s="55"/>
     </row>
-    <row r="36" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="93"/>
+    <row r="36" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="84"/>
       <c r="B36" s="23"/>
       <c r="G36" s="39"/>
       <c r="H36" s="39"/>
       <c r="I36" s="39"/>
-      <c r="J36" s="53"/>
+      <c r="J36" s="52"/>
       <c r="K36" s="40"/>
       <c r="L36" s="40"/>
       <c r="M36" s="40"/>
-      <c r="N36" s="56"/>
+      <c r="N36" s="55"/>
     </row>
-    <row r="37" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="93"/>
-      <c r="B37" s="136" t="s">
+    <row r="37" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="84"/>
+      <c r="B37" s="102" t="s">
         <v>86</v>
       </c>
-      <c r="C37" s="71" t="s">
+      <c r="C37" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="105" t="s">
+      <c r="D37" s="96" t="s">
         <v>73</v>
       </c>
-      <c r="E37" s="106" t="s">
+      <c r="E37" s="97" t="s">
         <v>74</v>
       </c>
-      <c r="F37" s="72" t="s">
+      <c r="F37" s="67" t="s">
         <v>75</v>
       </c>
       <c r="G37" s="39"/>
       <c r="H37" s="39"/>
-      <c r="I37" s="78" t="s">
+      <c r="I37" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="J37" s="137" t="s">
+      <c r="J37" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="K37" s="138"/>
-      <c r="L37" s="139"/>
+      <c r="K37" s="104"/>
+      <c r="L37" s="105"/>
       <c r="M37" s="39"/>
-      <c r="N37" s="56"/>
+      <c r="N37" s="55"/>
     </row>
-    <row r="38" spans="1:14" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="93"/>
-      <c r="B38" s="143"/>
-      <c r="C38" s="98" t="s">
+    <row r="38" spans="1:14" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A38" s="84"/>
+      <c r="B38" s="109"/>
+      <c r="C38" s="89" t="s">
         <v>72</v>
       </c>
-      <c r="D38" s="95" t="s">
+      <c r="D38" s="87" t="s">
         <v>76</v>
       </c>
-      <c r="E38" s="96" t="s">
+      <c r="E38" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="F38" s="95" t="s">
+      <c r="F38" s="87" t="s">
         <v>78</v>
       </c>
       <c r="G38" s="41"/>
       <c r="H38" s="41"/>
-      <c r="I38" s="78" t="s">
+      <c r="I38" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="J38" s="137" t="s">
+      <c r="J38" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="K38" s="138"/>
-      <c r="L38" s="139"/>
+      <c r="K38" s="104"/>
+      <c r="L38" s="105"/>
       <c r="M38" s="40"/>
-      <c r="N38" s="56"/>
+      <c r="N38" s="55"/>
     </row>
-    <row r="39" spans="1:14" s="45" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="93"/>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="84"/>
       <c r="M39" s="40"/>
-      <c r="N39" s="56"/>
+      <c r="N39" s="55"/>
     </row>
-    <row r="40" spans="1:14" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="93"/>
-      <c r="B40" s="140" t="s">
+    <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="84"/>
+      <c r="B40" s="106" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="140"/>
-      <c r="D40" s="140"/>
-      <c r="E40" s="140"/>
-      <c r="F40" s="140"/>
+      <c r="C40" s="106"/>
+      <c r="D40" s="106"/>
+      <c r="E40" s="106"/>
+      <c r="F40" s="106"/>
       <c r="G40" s="42"/>
       <c r="H40" s="39"/>
       <c r="I40" s="18"/>
@@ -31183,10 +31165,10 @@
       <c r="K40" s="38"/>
       <c r="L40" s="38"/>
       <c r="M40" s="39"/>
-      <c r="N40" s="56"/>
+      <c r="N40" s="55"/>
     </row>
-    <row r="41" spans="1:14" s="45" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="93"/>
+    <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="84"/>
       <c r="B41" s="111" t="s">
         <v>49</v>
       </c>
@@ -31201,10 +31183,10 @@
       <c r="K41" s="111"/>
       <c r="L41" s="111"/>
       <c r="M41" s="39"/>
-      <c r="N41" s="56"/>
+      <c r="N41" s="55"/>
     </row>
-    <row r="42" spans="1:14" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="93"/>
+    <row r="42" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="84"/>
       <c r="B42" s="111"/>
       <c r="C42" s="111"/>
       <c r="D42" s="111"/>
@@ -31217,10 +31199,10 @@
       <c r="K42" s="111"/>
       <c r="L42" s="111"/>
       <c r="M42" s="39"/>
-      <c r="N42" s="58"/>
+      <c r="N42" s="57"/>
     </row>
-    <row r="43" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A43" s="93"/>
+    <row r="43" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="84"/>
       <c r="B43" s="111"/>
       <c r="C43" s="111"/>
       <c r="D43" s="111"/>
@@ -31233,10 +31215,10 @@
       <c r="K43" s="111"/>
       <c r="L43" s="111"/>
       <c r="M43" s="39"/>
-      <c r="N43" s="58"/>
+      <c r="N43" s="57"/>
     </row>
-    <row r="44" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A44" s="93"/>
+    <row r="44" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="84"/>
       <c r="B44" s="111"/>
       <c r="C44" s="111"/>
       <c r="D44" s="111"/>
@@ -31249,10 +31231,10 @@
       <c r="K44" s="111"/>
       <c r="L44" s="111"/>
       <c r="M44" s="39"/>
-      <c r="N44" s="58"/>
+      <c r="N44" s="57"/>
     </row>
-    <row r="45" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="93"/>
+    <row r="45" spans="1:14" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A45" s="84"/>
       <c r="B45" s="111"/>
       <c r="C45" s="111"/>
       <c r="D45" s="111"/>
@@ -31264,11 +31246,11 @@
       <c r="J45" s="111"/>
       <c r="K45" s="111"/>
       <c r="L45" s="111"/>
-      <c r="M45" s="59"/>
-      <c r="N45" s="58"/>
+      <c r="M45" s="58"/>
+      <c r="N45" s="57"/>
     </row>
-    <row r="46" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A46" s="93"/>
+    <row r="46" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="84"/>
       <c r="B46" s="44"/>
       <c r="C46" s="39"/>
       <c r="D46" s="39"/>
@@ -31276,14 +31258,14 @@
       <c r="F46" s="39"/>
       <c r="G46" s="39"/>
       <c r="H46" s="39"/>
-      <c r="J46" s="52"/>
-      <c r="K46" s="52"/>
-      <c r="L46" s="52"/>
-      <c r="M46" s="59"/>
-      <c r="N46" s="58"/>
+      <c r="J46" s="51"/>
+      <c r="K46" s="51"/>
+      <c r="L46" s="51"/>
+      <c r="M46" s="58"/>
+      <c r="N46" s="57"/>
     </row>
-    <row r="47" spans="1:14" s="45" customFormat="1" ht="76.349999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="93"/>
+    <row r="47" spans="1:14" ht="76.349999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="84"/>
       <c r="B47" s="43"/>
       <c r="C47" s="39"/>
       <c r="D47" s="39"/>
@@ -31291,51 +31273,50 @@
       <c r="F47" s="39"/>
       <c r="G47" s="39"/>
       <c r="H47" s="39"/>
-      <c r="I47" s="68"/>
-      <c r="J47" s="66"/>
-      <c r="K47" s="66"/>
-      <c r="L47" s="69"/>
-      <c r="M47" s="59"/>
-      <c r="N47" s="58"/>
+      <c r="I47" s="23"/>
+      <c r="J47" s="62"/>
+      <c r="K47" s="62"/>
+      <c r="L47" s="64"/>
+      <c r="M47" s="58"/>
+      <c r="N47" s="57"/>
     </row>
-    <row r="48" spans="1:14" s="45" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A48" s="93"/>
+    <row r="48" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="84"/>
       <c r="B48" s="43"/>
-      <c r="C48" s="54"/>
+      <c r="C48" s="53"/>
       <c r="D48" s="17"/>
       <c r="E48" s="17"/>
-      <c r="F48" s="55"/>
-      <c r="G48" s="55"/>
-      <c r="H48" s="87"/>
-      <c r="I48" s="86"/>
-      <c r="J48" s="88"/>
-      <c r="K48" s="85"/>
-      <c r="L48" s="69"/>
-      <c r="M48" s="59"/>
-      <c r="N48" s="58"/>
+      <c r="F48" s="54"/>
+      <c r="G48" s="54"/>
+      <c r="H48" s="81"/>
+      <c r="I48" s="80"/>
+      <c r="J48" s="82"/>
+      <c r="L48" s="64"/>
+      <c r="M48" s="58"/>
+      <c r="N48" s="57"/>
     </row>
-    <row r="49" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="90"/>
+    <row r="49" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="84"/>
       <c r="B49" s="13"/>
-      <c r="C49" s="134" t="s">
+      <c r="C49" s="100" t="s">
         <v>111</v>
       </c>
-      <c r="D49" s="135"/>
-      <c r="E49" s="135"/>
+      <c r="D49" s="101"/>
+      <c r="E49" s="101"/>
       <c r="F49" s="12"/>
       <c r="G49" s="12"/>
-      <c r="H49" s="141" t="s">
+      <c r="H49" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="I49" s="141"/>
-      <c r="J49" s="141"/>
+      <c r="I49" s="107"/>
+      <c r="J49" s="107"/>
       <c r="K49" s="12"/>
       <c r="L49" s="12"/>
       <c r="M49" s="12"/>
       <c r="N49" s="11"/>
     </row>
-    <row r="50" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="94"/>
+    <row r="50" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="86"/>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
@@ -31352,6 +31333,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="A1:C5"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="D1:J5"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="I26:L26"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
     <mergeCell ref="B16:B18"/>
     <mergeCell ref="C49:E49"/>
     <mergeCell ref="J27:J28"/>
@@ -31366,30 +31365,12 @@
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="I25:L25"/>
     <mergeCell ref="B41:L45"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="I26:L26"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="A1:C5"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="D1:J5"/>
-    <mergeCell ref="G14:G15"/>
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="K3:N3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.55118110236220474" bottom="0.35433070866141736" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="63" fitToWidth="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="64" fitToWidth="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>